<commit_message>
Adding Benchmarks of Grover's and Amplitude Estimation performed on IONQ simulators
</commit_message>
<xml_diff>
--- a/CLOUD/IONQ/Deutsch-Jozsa/Deutsch-Jozsa Benchmark-Results.xlsx
+++ b/CLOUD/IONQ/Deutsch-Jozsa/Deutsch-Jozsa Benchmark-Results.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,6 +453,24 @@
           <t>Qiskit-IONQ: Algorithm = Deutsch-Jozsa Simulator = ionq_simulator-0.0.1--ideal</t>
         </is>
       </c>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="n"/>
+      <c r="S2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -460,6 +478,24 @@
           <t>CLOUD SIMULATOR - Maximum Supported qubits:29</t>
         </is>
       </c>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="1" t="n"/>
+      <c r="F3" s="1" t="n"/>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+      <c r="K3" s="1" t="n"/>
+      <c r="L3" s="1" t="n"/>
+      <c r="M3" s="1" t="n"/>
+      <c r="N3" s="1" t="n"/>
+      <c r="O3" s="1" t="n"/>
+      <c r="P3" s="1" t="n"/>
+      <c r="Q3" s="1" t="n"/>
+      <c r="R3" s="1" t="n"/>
+      <c r="S3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -467,876 +503,1564 @@
           <t>Configuration: Min_Qubits = 3 Max_Qubits = 28 Skip_Qubits = 2 num_circuits = 2  QV_ = None Last_Updated = 2024-09-06 11:37:07</t>
         </is>
       </c>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+      <c r="E4" s="1" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+      <c r="K4" s="1" t="n"/>
+      <c r="L4" s="1" t="n"/>
+      <c r="M4" s="1" t="n"/>
+      <c r="N4" s="1" t="n"/>
+      <c r="O4" s="1" t="n"/>
+      <c r="P4" s="1" t="n"/>
+      <c r="Q4" s="1" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>Number of Qubits</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>avg_creation_times (ms)</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>std_creation_times (ms)</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>avg_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>std_elapsed_times (ms)</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="1" t="inlineStr">
         <is>
           <t>avg_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="1" t="inlineStr">
         <is>
           <t>std_quantum_times (ms)</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="1" t="inlineStr">
         <is>
           <t>avg_circuit_depths</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="1" t="inlineStr">
         <is>
           <t>avg_transpiled_depths</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="J5" s="1" t="inlineStr">
         <is>
           <t>Average_Rescaled_fidelity</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="K5" s="1" t="inlineStr">
         <is>
           <t>Average_Hellinger_fidelity</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="1" t="inlineStr">
         <is>
           <t>std_Rescaled_Fidelity</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="M5" s="1" t="inlineStr">
         <is>
           <t>std_hellinger_fidelity</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="N5" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="O5" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_algorithmic_gate_counts</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P5" s="1" t="inlineStr">
         <is>
           <t>avg_xi (n2q/n1q+n2q)</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q5" s="1" t="inlineStr">
         <is>
           <t>avg_1Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R5" s="1" t="inlineStr">
         <is>
           <t>avg_2Q_Transpiled_gate_counts</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S5" s="1" t="inlineStr">
         <is>
           <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="1" t="n">
         <v>6.504</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.203</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" s="1" t="n">
         <v>7400.728</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="1" t="n">
         <v>98.53400000000001</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="1" t="n">
         <v>23.534</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
+      <c r="J6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="O6" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="Q6" t="n">
+      <c r="O6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q6" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="R6" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" t="n">
+      <c r="R6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1" t="n">
         <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="1" t="n">
         <v>3.947</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.5580000000000001</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="1" t="n">
         <v>8251.882</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="1" t="n">
         <v>284.058</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="1" t="n">
         <v>0.588</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
+      <c r="J7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1" t="n">
         <v>14.5</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="P7" t="n">
+      <c r="P7" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" s="1" t="n">
         <v>20.5</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S7" t="n">
+      <c r="S7" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="1" t="n">
         <v>11.748</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.89</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" s="1" t="n">
         <v>7796.434</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="1" t="n">
         <v>187.169</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="1" t="n">
         <v>0.196</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="1" t="n">
         <v>9.5</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="1" t="n">
         <v>9.5</v>
       </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
+      <c r="J8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1" t="n">
         <v>19.5</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="P8" t="n">
+      <c r="P8" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" s="1" t="n">
         <v>29.5</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="S8" t="n">
+      <c r="S8" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.403</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" s="1" t="n">
         <v>7879.91</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="1" t="n">
         <v>57.185</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.196</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
+      <c r="J9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="P9" t="n">
+      <c r="P9" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="S9" t="n">
+      <c r="S9" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="1" t="n">
         <v>11.486</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.328</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" s="1" t="n">
         <v>6948.431</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="1" t="n">
         <v>12.255</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="1" t="n">
         <v>376</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="1" t="n">
         <v>70.20999999999999</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" s="1" t="n">
         <v>11.5</v>
       </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="n">
         <v>29.5</v>
       </c>
-      <c r="O10" t="n">
+      <c r="O10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="P10" t="n">
+      <c r="P10" s="1" t="n">
         <v>0.11</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Q10" s="1" t="n">
         <v>47.5</v>
       </c>
-      <c r="R10" t="n">
+      <c r="R10" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S10" t="n">
+      <c r="S10" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="1" t="n">
         <v>3.902</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" s="1" t="n">
         <v>0.438</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" s="1" t="n">
         <v>7060.085</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="1" t="n">
         <v>40.149</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11" s="1" t="n">
         <v>319</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" s="1" t="n">
         <v>59.031</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="1" t="n">
         <v>12.5</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="1" t="n">
         <v>12.5</v>
       </c>
-      <c r="J11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
+      <c r="J11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1" t="n">
         <v>34.5</v>
       </c>
-      <c r="O11" t="n">
+      <c r="O11" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="P11" t="n">
+      <c r="P11" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Q11" s="1" t="n">
         <v>56.5</v>
       </c>
-      <c r="R11" t="n">
+      <c r="R11" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="S11" t="n">
+      <c r="S11" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="1" t="n">
         <v>7.479</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.206</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" s="1" t="n">
         <v>6873.713</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="1" t="n">
         <v>0.607</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12" s="1" t="n">
         <v>31.5</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="1" t="n">
         <v>0.294</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="1" t="n">
         <v>13.5</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" s="1" t="n">
         <v>13.5</v>
       </c>
-      <c r="J12" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
+      <c r="J12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="n">
         <v>39.5</v>
       </c>
-      <c r="O12" t="n">
+      <c r="O12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="P12" t="n">
+      <c r="P12" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="Q12" s="1" t="n">
         <v>65.5</v>
       </c>
-      <c r="R12" t="n">
+      <c r="R12" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="S12" t="n">
+      <c r="S12" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="1" t="n">
         <v>4.125</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.376</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="1" t="n">
         <v>7459.568</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="1" t="n">
         <v>22.775</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="1" t="n">
         <v>709.5</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="1" t="n">
         <v>1.667</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="1" t="n">
         <v>14.5</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" s="1" t="n">
         <v>14.5</v>
       </c>
-      <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
+      <c r="J13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="n">
         <v>44.5</v>
       </c>
-      <c r="O13" t="n">
+      <c r="O13" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="P13" t="n">
+      <c r="P13" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="Q13" s="1" t="n">
         <v>74.5</v>
       </c>
-      <c r="R13" t="n">
+      <c r="R13" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="S13" t="n">
+      <c r="S13" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="1" t="n">
         <v>4.365</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.332</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="1" t="n">
         <v>8071.428</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="1" t="n">
         <v>136.813</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="1" t="n">
         <v>829</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" s="1" t="n">
         <v>4.511</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14" s="1" t="n">
         <v>15.5</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" s="1" t="n">
         <v>15.5</v>
       </c>
-      <c r="J14" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" t="n">
-        <v>1</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
+      <c r="J14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1" t="n">
         <v>49.5</v>
       </c>
-      <c r="O14" t="n">
+      <c r="O14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="P14" t="n">
+      <c r="P14" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q14" s="1" t="n">
         <v>83.5</v>
       </c>
-      <c r="R14" t="n">
+      <c r="R14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="S14" t="n">
+      <c r="S14" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n">
+      <c r="A15" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="1" t="n">
         <v>7.212</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.204</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="1" t="n">
         <v>7830.688</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" s="1" t="n">
         <v>187.434</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15" s="1" t="n">
         <v>1231</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15" s="1" t="n">
         <v>3.726</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" s="1" t="n">
         <v>16.5</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" s="1" t="n">
         <v>16.5</v>
       </c>
-      <c r="J15" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
+      <c r="J15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="O15" t="n">
+      <c r="O15" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="P15" t="n">
+      <c r="P15" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="Q15" s="1" t="n">
         <v>92.5</v>
       </c>
-      <c r="R15" t="n">
+      <c r="R15" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S15" t="n">
+      <c r="S15" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
+      <c r="A16" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="1" t="n">
         <v>11.665</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="1" t="n">
         <v>0.233</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="1" t="n">
         <v>7208.385</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="1" t="n">
         <v>52.937</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16" s="1" t="n">
         <v>3019.5</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" s="1" t="n">
         <v>5.001</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16" s="1" t="n">
         <v>17.5</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" s="1" t="n">
         <v>17.5</v>
       </c>
-      <c r="J16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
+      <c r="J16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1" t="n">
         <v>59.5</v>
       </c>
-      <c r="O16" t="n">
+      <c r="O16" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="P16" t="n">
+      <c r="P16" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="Q16" s="1" t="n">
         <v>101.5</v>
       </c>
-      <c r="R16" t="n">
+      <c r="R16" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="S16" t="n">
+      <c r="S16" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
+      <c r="A17" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" s="1" t="n">
         <v>12.589</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="1" t="n">
         <v>0.107</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="1" t="n">
         <v>15100.532</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="1" t="n">
         <v>513.371</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17" s="1" t="n">
         <v>10461</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17" s="1" t="n">
         <v>47.656</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="J17" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
-      <c r="N17" t="n">
+      <c r="J17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="O17" t="n">
+      <c r="O17" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="P17" t="n">
+      <c r="P17" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="Q17" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="R17" t="n">
+      <c r="R17" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="S17" t="n">
+      <c r="S17" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n">
+      <c r="A18" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="1" t="n">
         <v>7.956</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="1" t="n">
         <v>0.437</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="1" t="n">
         <v>48355.075</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="1" t="n">
         <v>546.048</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="1" t="n">
         <v>42460</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="1" t="n">
         <v>254.363</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="J18" t="n">
-        <v>1</v>
-      </c>
-      <c r="K18" t="n">
-        <v>1</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
+      <c r="J18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="O18" t="n">
+      <c r="O18" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="P18" t="n">
+      <c r="P18" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="Q18" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="R18" t="n">
+      <c r="R18" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="S18" t="n">
-        <v>0.08</v>
-      </c>
+      <c r="S18" s="1" t="n">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr"/>
+      <c r="B19" s="1" t="inlineStr"/>
+      <c r="C19" s="1" t="inlineStr"/>
+      <c r="D19" s="1" t="inlineStr"/>
+      <c r="E19" s="1" t="inlineStr"/>
+      <c r="F19" s="1" t="inlineStr"/>
+      <c r="G19" s="1" t="inlineStr"/>
+      <c r="H19" s="1" t="inlineStr"/>
+      <c r="I19" s="1" t="inlineStr"/>
+      <c r="J19" s="1" t="inlineStr"/>
+      <c r="K19" s="1" t="inlineStr"/>
+      <c r="L19" s="1" t="inlineStr"/>
+      <c r="M19" s="1" t="inlineStr"/>
+      <c r="N19" s="1" t="inlineStr"/>
+      <c r="O19" s="1" t="inlineStr"/>
+      <c r="P19" s="1" t="inlineStr"/>
+      <c r="Q19" s="1" t="inlineStr"/>
+      <c r="R19" s="1" t="inlineStr"/>
+      <c r="S19" s="1" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit-IONQ: Algorithm = Deutsch-Jozsa Simulator = ionq_simulator-0.0.1--ideal</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n"/>
+      <c r="C20" s="1" t="n"/>
+      <c r="D20" s="1" t="n"/>
+      <c r="E20" s="1" t="n"/>
+      <c r="F20" s="1" t="n"/>
+      <c r="G20" s="1" t="n"/>
+      <c r="H20" s="1" t="n"/>
+      <c r="I20" s="1" t="n"/>
+      <c r="J20" s="1" t="n"/>
+      <c r="K20" s="1" t="n"/>
+      <c r="L20" s="1" t="n"/>
+      <c r="M20" s="1" t="n"/>
+      <c r="N20" s="1" t="n"/>
+      <c r="O20" s="1" t="n"/>
+      <c r="P20" s="1" t="n"/>
+      <c r="Q20" s="1" t="n"/>
+      <c r="R20" s="1" t="n"/>
+      <c r="S20" s="1" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>CLOUD SIMULATOR - Maximum Supported qubits:29</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="n"/>
+      <c r="C21" s="1" t="n"/>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n"/>
+      <c r="F21" s="1" t="n"/>
+      <c r="G21" s="1" t="n"/>
+      <c r="H21" s="1" t="n"/>
+      <c r="I21" s="1" t="n"/>
+      <c r="J21" s="1" t="n"/>
+      <c r="K21" s="1" t="n"/>
+      <c r="L21" s="1" t="n"/>
+      <c r="M21" s="1" t="n"/>
+      <c r="N21" s="1" t="n"/>
+      <c r="O21" s="1" t="n"/>
+      <c r="P21" s="1" t="n"/>
+      <c r="Q21" s="1" t="n"/>
+      <c r="R21" s="1" t="n"/>
+      <c r="S21" s="1" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 3 Max_Qubits = 4 Skip_Qubits = 1 num_circuits = 2  QV_ = None Last_Updated = 2024-09-09 12:05:19</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n"/>
+      <c r="C22" s="1" t="n"/>
+      <c r="D22" s="1" t="n"/>
+      <c r="E22" s="1" t="n"/>
+      <c r="F22" s="1" t="n"/>
+      <c r="G22" s="1" t="n"/>
+      <c r="H22" s="1" t="n"/>
+      <c r="I22" s="1" t="n"/>
+      <c r="J22" s="1" t="n"/>
+      <c r="K22" s="1" t="n"/>
+      <c r="L22" s="1" t="n"/>
+      <c r="M22" s="1" t="n"/>
+      <c r="N22" s="1" t="n"/>
+      <c r="O22" s="1" t="n"/>
+      <c r="P22" s="1" t="n"/>
+      <c r="Q22" s="1" t="n"/>
+      <c r="R22" s="1" t="n"/>
+      <c r="S22" s="1" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F23" s="1" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G23" s="1" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H23" s="1" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I23" s="1" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J23" s="1" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K23" s="1" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L23" s="1" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M23" s="1" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N23" s="1" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O23" s="1" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P23" s="1" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q23" s="1" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R23" s="1" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S23" s="1" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>7.353</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>2.674</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>7130.367</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>96.111</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q24" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="R24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>7.726</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>4675.46</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>1122.592</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P25" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="S25" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr"/>
+      <c r="B26" s="1" t="inlineStr"/>
+      <c r="C26" s="1" t="inlineStr"/>
+      <c r="D26" s="1" t="inlineStr"/>
+      <c r="E26" s="1" t="inlineStr"/>
+      <c r="F26" s="1" t="inlineStr"/>
+      <c r="G26" s="1" t="inlineStr"/>
+      <c r="H26" s="1" t="inlineStr"/>
+      <c r="I26" s="1" t="inlineStr"/>
+      <c r="J26" s="1" t="inlineStr"/>
+      <c r="K26" s="1" t="inlineStr"/>
+      <c r="L26" s="1" t="inlineStr"/>
+      <c r="M26" s="1" t="inlineStr"/>
+      <c r="N26" s="1" t="inlineStr"/>
+      <c r="O26" s="1" t="inlineStr"/>
+      <c r="P26" s="1" t="inlineStr"/>
+      <c r="Q26" s="1" t="inlineStr"/>
+      <c r="R26" s="1" t="inlineStr"/>
+      <c r="S26" s="1" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr"/>
+      <c r="B27" s="1" t="inlineStr"/>
+      <c r="C27" s="1" t="inlineStr"/>
+      <c r="D27" s="1" t="inlineStr"/>
+      <c r="E27" s="1" t="inlineStr"/>
+      <c r="F27" s="1" t="inlineStr"/>
+      <c r="G27" s="1" t="inlineStr"/>
+      <c r="H27" s="1" t="inlineStr"/>
+      <c r="I27" s="1" t="inlineStr"/>
+      <c r="J27" s="1" t="inlineStr"/>
+      <c r="K27" s="1" t="inlineStr"/>
+      <c r="L27" s="1" t="inlineStr"/>
+      <c r="M27" s="1" t="inlineStr"/>
+      <c r="N27" s="1" t="inlineStr"/>
+      <c r="O27" s="1" t="inlineStr"/>
+      <c r="P27" s="1" t="inlineStr"/>
+      <c r="Q27" s="1" t="inlineStr"/>
+      <c r="R27" s="1" t="inlineStr"/>
+      <c r="S27" s="1" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Qiskit-IONQ: Algorithm = Deutsch-Jozsa Simulator = ionq_simulator-0.0.1--ideal</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="1" t="n"/>
+      <c r="D28" s="1" t="n"/>
+      <c r="E28" s="1" t="n"/>
+      <c r="F28" s="1" t="n"/>
+      <c r="G28" s="1" t="n"/>
+      <c r="H28" s="1" t="n"/>
+      <c r="I28" s="1" t="n"/>
+      <c r="J28" s="1" t="n"/>
+      <c r="K28" s="1" t="n"/>
+      <c r="L28" s="1" t="n"/>
+      <c r="M28" s="1" t="n"/>
+      <c r="N28" s="1" t="n"/>
+      <c r="O28" s="1" t="n"/>
+      <c r="P28" s="1" t="n"/>
+      <c r="Q28" s="1" t="n"/>
+      <c r="R28" s="1" t="n"/>
+      <c r="S28" s="1" t="n"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>CLOUD SIMULATOR - Maximum Supported qubits:29</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="n"/>
+      <c r="D29" s="1" t="n"/>
+      <c r="E29" s="1" t="n"/>
+      <c r="F29" s="1" t="n"/>
+      <c r="G29" s="1" t="n"/>
+      <c r="H29" s="1" t="n"/>
+      <c r="I29" s="1" t="n"/>
+      <c r="J29" s="1" t="n"/>
+      <c r="K29" s="1" t="n"/>
+      <c r="L29" s="1" t="n"/>
+      <c r="M29" s="1" t="n"/>
+      <c r="N29" s="1" t="n"/>
+      <c r="O29" s="1" t="n"/>
+      <c r="P29" s="1" t="n"/>
+      <c r="Q29" s="1" t="n"/>
+      <c r="R29" s="1" t="n"/>
+      <c r="S29" s="1" t="n"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Configuration: Min_Qubits = 3 Max_Qubits = 4 Skip_Qubits = 1 num_circuits = 2  QV_ = None Last_Updated = 2024-09-09 12:11:27</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n"/>
+      <c r="C30" s="1" t="n"/>
+      <c r="D30" s="1" t="n"/>
+      <c r="E30" s="1" t="n"/>
+      <c r="F30" s="1" t="n"/>
+      <c r="G30" s="1" t="n"/>
+      <c r="H30" s="1" t="n"/>
+      <c r="I30" s="1" t="n"/>
+      <c r="J30" s="1" t="n"/>
+      <c r="K30" s="1" t="n"/>
+      <c r="L30" s="1" t="n"/>
+      <c r="M30" s="1" t="n"/>
+      <c r="N30" s="1" t="n"/>
+      <c r="O30" s="1" t="n"/>
+      <c r="P30" s="1" t="n"/>
+      <c r="Q30" s="1" t="n"/>
+      <c r="R30" s="1" t="n"/>
+      <c r="S30" s="1" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Number of Qubits</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>avg_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>std_creation_times (ms)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>avg_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>std_elapsed_times (ms)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>avg_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>std_quantum_times (ms)</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>avg_circuit_depths</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>avg_transpiled_depths</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Average_Rescaled_fidelity</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Average_Hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>std_Rescaled_Fidelity</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>std_hellinger_fidelity</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>avg_1Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>avg_2Q_algorithmic_gate_counts</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>avg_xi (n2q/n1q+n2q)</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>avg_1Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>avg_2Q_Transpiled_gate_counts</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>avg_tr_xi (tr_n2q/tr_n1q+tr_n2q)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3</v>
+      </c>
+      <c r="B32" t="n">
+        <v>7.165</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.857</v>
+      </c>
+      <c r="D32" t="n">
+        <v>7633.599</v>
+      </c>
+      <c r="E32" t="n">
+        <v>293.911</v>
+      </c>
+      <c r="F32" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="G32" t="n">
+        <v>37.75</v>
+      </c>
+      <c r="H32" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="R32" t="n">
+        <v>1</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" t="n">
+        <v>9.329000000000001</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.771</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7473.768</v>
+      </c>
+      <c r="E33" t="n">
+        <v>97.643</v>
+      </c>
+      <c r="F33" t="n">
+        <v>191.5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>87.75</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="I33" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>12</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>16</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="A28:S28"/>
+    <mergeCell ref="A22:S22"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A21:S21"/>
     <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A20:S20"/>
+    <mergeCell ref="A30:S30"/>
     <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A29:S29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1348,7 +2072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2859,7 +3583,6 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="30"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:S4"/>
@@ -2877,7 +3600,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S16"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2912,24 +3635,6 @@
           <t>Qiskit-IONQ: Algorithm = Deutsch-Jozsa Simulator = ionq_simulator-0.0.1--harmony-1</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2937,24 +3642,6 @@
           <t>CLOUD SIMULATOR - Maximum Supported qubits:29</t>
         </is>
       </c>
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
-      <c r="D3" s="1" t="n"/>
-      <c r="E3" s="1" t="n"/>
-      <c r="F3" s="1" t="n"/>
-      <c r="G3" s="1" t="n"/>
-      <c r="H3" s="1" t="n"/>
-      <c r="I3" s="1" t="n"/>
-      <c r="J3" s="1" t="n"/>
-      <c r="K3" s="1" t="n"/>
-      <c r="L3" s="1" t="n"/>
-      <c r="M3" s="1" t="n"/>
-      <c r="N3" s="1" t="n"/>
-      <c r="O3" s="1" t="n"/>
-      <c r="P3" s="1" t="n"/>
-      <c r="Q3" s="1" t="n"/>
-      <c r="R3" s="1" t="n"/>
-      <c r="S3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2962,24 +3649,6 @@
           <t>Executing with Noise</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n"/>
-      <c r="C4" s="1" t="n"/>
-      <c r="D4" s="1" t="n"/>
-      <c r="E4" s="1" t="n"/>
-      <c r="F4" s="1" t="n"/>
-      <c r="G4" s="1" t="n"/>
-      <c r="H4" s="1" t="n"/>
-      <c r="I4" s="1" t="n"/>
-      <c r="J4" s="1" t="n"/>
-      <c r="K4" s="1" t="n"/>
-      <c r="L4" s="1" t="n"/>
-      <c r="M4" s="1" t="n"/>
-      <c r="N4" s="1" t="n"/>
-      <c r="O4" s="1" t="n"/>
-      <c r="P4" s="1" t="n"/>
-      <c r="Q4" s="1" t="n"/>
-      <c r="R4" s="1" t="n"/>
-      <c r="S4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2987,24 +3656,6 @@
           <t>Configuration: Min_Qubits = 3 Max_Qubits = 11 Skip_Qubits = 1 num_circuits = 2  QV_ = None Last_Updated = 2024-09-06 12:46:52</t>
         </is>
       </c>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n"/>
-      <c r="E5" s="1" t="n"/>
-      <c r="F5" s="1" t="n"/>
-      <c r="G5" s="1" t="n"/>
-      <c r="H5" s="1" t="n"/>
-      <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="n"/>
-      <c r="K5" s="1" t="n"/>
-      <c r="L5" s="1" t="n"/>
-      <c r="M5" s="1" t="n"/>
-      <c r="N5" s="1" t="n"/>
-      <c r="O5" s="1" t="n"/>
-      <c r="P5" s="1" t="n"/>
-      <c r="Q5" s="1" t="n"/>
-      <c r="R5" s="1" t="n"/>
-      <c r="S5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3633,27 +4284,6 @@
       <c r="S15" t="n">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>